<commit_message>
Added PEB and Protection offsets
</commit_message>
<xml_diff>
--- a/offsets.xlsx
+++ b/offsets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\worker\Documents\GitHub\eprocess_offsets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/worker/Documents/Github/eprocess_offsets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064A1785-11BC-4A01-9024-27C7BC57212A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B98C970-2CD9-B54F-8977-D835DE54102F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15990" yWindow="360" windowWidth="14790" windowHeight="14205" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35040" yWindow="-9600" windowWidth="33840" windowHeight="19360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
   <si>
     <t>Windows Version</t>
   </si>
@@ -133,13 +133,46 @@
   </si>
   <si>
     <t>0x1d0</t>
+  </si>
+  <si>
+    <t>Windows 10 22H2</t>
+  </si>
+  <si>
+    <t>PEB</t>
+  </si>
+  <si>
+    <t>Protection</t>
+  </si>
+  <si>
+    <t>0x5fa</t>
+  </si>
+  <si>
+    <t>0x550</t>
+  </si>
+  <si>
+    <t>0x87a</t>
+  </si>
+  <si>
+    <t>0x3f8</t>
+  </si>
+  <si>
+    <t>0x6fa</t>
+  </si>
+  <si>
+    <t>0x6ca</t>
+  </si>
+  <si>
+    <t>0x6c2</t>
+  </si>
+  <si>
+    <t>0x6aa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -147,12 +180,31 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +247,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -225,30 +283,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -273,56 +311,49 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -406,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -446,7 +477,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -552,7 +583,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -722,21 +753,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -749,351 +780,527 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>26200</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="1">
         <v>26100</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="20"/>
+    </row>
+    <row r="4" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>22631</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="F4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>22621</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="F5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>20348</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="F6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>22000</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="F7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1">
         <v>22000</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="F8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
+        <v>19045</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
+        <v>19044</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>19043</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>19042</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
         <v>19041</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E13" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1">
-        <v>19041</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1">
-        <v>19041</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1">
-        <v>19041</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="F13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="1">
-        <v>18362</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>18362</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="F14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18362</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>17763</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E16" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="F16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>17134</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E17" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="F17" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>16299</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E18" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="F18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>15063</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E19" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="F19" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>14393</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E20" s="17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="F20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>10586</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E21" s="17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="F21" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:8" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B22" s="11">
         <v>10240</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D22" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E22" s="21" t="s">
         <v>19</v>
       </c>
+      <c r="F22" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>

</xml_diff>